<commit_message>
Refined app to remove folders on restart, prevent file generation on all server connection failures, and display an error message
</commit_message>
<xml_diff>
--- a/server_template.xlsx
+++ b/server_template.xlsx
@@ -784,13 +784,13 @@
         <v>45</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.1939</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>45</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.454545</v>
+        <v>0.649351</v>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="5">
@@ -809,13 +809,13 @@
         <v>50</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.1939</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>50</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.454545</v>
+        <v>0.649351</v>
       </c>
     </row>
     <row r="4"/>

</xml_diff>